<commit_message>
Update Files on MeetOpt
</commit_message>
<xml_diff>
--- a/Variables_and_Assumptions.xlsx
+++ b/Variables_and_Assumptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdb025\Documents\Research\Maciek\Swim Models 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdb025\Documents\GitHub\MeetOpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>MaxSolveTime</t>
   </si>
@@ -195,9 +195,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>This is for VORP and tells the model if you want to include all the athletes for the all the events. I've set this to "ALL" for now. Only needed if we uncomment the VORP/WAR section</t>
-  </si>
-  <si>
     <t>HomeAthPredTime</t>
   </si>
   <si>
@@ -244,6 +241,54 @@
   </si>
   <si>
     <t>Print statements need to be updated for Python 3</t>
+  </si>
+  <si>
+    <t>indivplcscore</t>
+  </si>
+  <si>
+    <t>relayplcscore</t>
+  </si>
+  <si>
+    <t>List of points for finishing places in INDIVIDUAL events</t>
+  </si>
+  <si>
+    <t>List of points for finishing places in RELAY events</t>
+  </si>
+  <si>
+    <t>This is for VORP and tells the model if you want to include all the athletes for the all the events. Only needed if we uncomment the VORP/WAR section</t>
+  </si>
+  <si>
+    <t>playperf</t>
+  </si>
+  <si>
+    <t>playperfstart</t>
+  </si>
+  <si>
+    <t>playperfMR</t>
+  </si>
+  <si>
+    <t>athlete, stroke</t>
+  </si>
+  <si>
+    <t>athlete, relaynoMR</t>
+  </si>
+  <si>
+    <t>athlete, indiv</t>
+  </si>
+  <si>
+    <t>pred times for each athlete in each individual event</t>
+  </si>
+  <si>
+    <t>TopopprankIndiv</t>
+  </si>
+  <si>
+    <t>TopopprankRelay</t>
+  </si>
+  <si>
+    <t>Currently 3, the number of opponents assigned to each INDIVIDUAL. In non-dual meets, you could have as many as 5 other opponents in a race</t>
+  </si>
+  <si>
+    <t>Currently 3, the number of opponents in each relay event. In non-dual meets, you could have as many as 5 other opponents in a race</t>
   </si>
 </sst>
 </file>
@@ -570,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -725,49 +770,43 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -776,12 +815,12 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -790,12 +829,12 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -804,137 +843,229 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
         <v>68</v>
       </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D35" t="s">
         <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>